<commit_message>
- move VCC track away from M4 hole - exchange 383k resistors by E12 390k - use 10k resistors for VGND providers (quicker startup)
</commit_message>
<xml_diff>
--- a/Preamp/Vuvlo_calc.xlsx
+++ b/Preamp/Vuvlo_calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="60" windowWidth="10884" windowHeight="4800" activeTab="1"/>
+    <workbookView xWindow="384" yWindow="60" windowWidth="10884" windowHeight="4800"/>
   </bookViews>
   <sheets>
     <sheet name="PowerConditioner" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -158,7 +158,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1608,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1654,7 +1654,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>383</v>
+        <v>390</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1702,22 +1702,22 @@
       </c>
       <c r="D10" s="1">
         <f>$B$5*$B$6/C10</f>
-        <v>51.066666666666663</v>
+        <v>52</v>
       </c>
       <c r="E10">
         <f>D10/B12</f>
-        <v>10.213333333333333</v>
+        <v>10.4</v>
       </c>
       <c r="F10">
         <v>50</v>
       </c>
       <c r="G10" s="1">
         <f>$B$6*1/(F10/$B$5)</f>
-        <v>9.1919999999999984</v>
+        <v>9.3600000000000012</v>
       </c>
       <c r="H10">
         <f>G10/B10</f>
-        <v>3.0639999999999996</v>
+        <v>3.1200000000000006</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1732,22 +1732,22 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11:D12" si="0">$B$5*$B$6/C11</f>
-        <v>38.299999999999997</v>
+        <v>39</v>
       </c>
       <c r="E11">
         <f>D11/B11</f>
-        <v>9.5749999999999993</v>
+        <v>9.75</v>
       </c>
       <c r="F11">
         <v>40</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" ref="G11:G12" si="1">$B$6*1/(F11/$B$5)</f>
-        <v>11.49</v>
+        <v>11.7</v>
       </c>
       <c r="H11">
         <f>G11/B11</f>
-        <v>2.8725000000000001</v>
+        <v>2.9249999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1762,22 +1762,22 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>30.639999999999997</v>
+        <v>31.2</v>
       </c>
       <c r="E12">
         <f>D12/B10</f>
-        <v>10.213333333333333</v>
+        <v>10.4</v>
       </c>
       <c r="F12">
         <v>30</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>15.319999999999999</v>
+        <v>15.599999999999998</v>
       </c>
       <c r="H12">
         <f>G12/B12</f>
-        <v>3.0639999999999996</v>
+        <v>3.1199999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1813,7 +1813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- Change from EH to XH connectors, vertical - Re-align and place connectors - Delete LED, use TestPoint instead - Optimize 2mm tracks for shortness - update BOM
</commit_message>
<xml_diff>
--- a/Preamp/Vuvlo_calc.xlsx
+++ b/Preamp/Vuvlo_calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="60" windowWidth="10884" windowHeight="4800"/>
+    <workbookView xWindow="384" yWindow="60" windowWidth="10884" windowHeight="4800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PowerConditioner" sheetId="1" r:id="rId1"/>
@@ -108,10 +108,10 @@
     <t>16v</t>
   </si>
   <si>
-    <t>2* 22u</t>
-  </si>
-  <si>
     <t>R2 chosen</t>
+  </si>
+  <si>
+    <t>2* 47u</t>
   </si>
 </sst>
 </file>
@@ -1608,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1681,7 +1681,7 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -1813,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1870,7 +1870,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
- update 1.25k resistors to 1.2k resistors
</commit_message>
<xml_diff>
--- a/Preamp/Vuvlo_calc.xlsx
+++ b/Preamp/Vuvlo_calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="60" windowWidth="10884" windowHeight="4800" activeTab="1"/>
+    <workbookView xWindow="384" yWindow="60" windowWidth="10884" windowHeight="4800"/>
   </bookViews>
   <sheets>
     <sheet name="PowerConditioner" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Vuvlo = Vbg * 1/(R1/R2)</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>2* 47u</t>
+  </si>
+  <si>
+    <t>SETI</t>
+  </si>
+  <si>
+    <t>2.4kOhm</t>
   </si>
 </sst>
 </file>
@@ -1606,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1800,6 +1806,16 @@
       </c>
       <c r="C15" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1813,8 +1829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1843,7 +1859,7 @@
       </c>
       <c r="B4">
         <f>B3/(B6-1)</f>
-        <v>1.25</v>
+        <v>1.2004801920768307</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1851,7 +1867,7 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>9.33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add logos to solution /2D update Max1756c calculation update 3D data for CNC
</commit_message>
<xml_diff>
--- a/Preamp/Vuvlo_calc.xlsx
+++ b/Preamp/Vuvlo_calc.xlsx
@@ -1612,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1623,7 +1623,7 @@
     <col min="5" max="5" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1634,12 +1634,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1674,12 +1674,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1715,18 +1715,18 @@
         <v>10.4</v>
       </c>
       <c r="F10">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G10" s="1">
-        <f>$B$6*1/(F10/$B$5)</f>
-        <v>9.3600000000000012</v>
+        <f>$B$6*(1 + $B$5/F10)</f>
+        <v>10.030188679245283</v>
       </c>
       <c r="H10">
         <f>G10/B10</f>
-        <v>3.1200000000000006</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>3.3433962264150945</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1745,18 +1745,19 @@
         <v>9.75</v>
       </c>
       <c r="F11">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" ref="G11:G12" si="1">$B$6*1/(F11/$B$5)</f>
-        <v>11.7</v>
+        <f t="shared" ref="G11:G12" si="1">$B$6*(1 + $B$5/F11)</f>
+        <v>12.083720930232557</v>
       </c>
       <c r="H11">
         <f>G11/B11</f>
-        <v>2.9249999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>3.0209302325581393</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1775,18 +1776,19 @@
         <v>10.4</v>
       </c>
       <c r="F12">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>15.599999999999998</v>
+        <v>15.381818181818181</v>
       </c>
       <c r="H12">
         <f>G12/B12</f>
-        <v>3.1199999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>3.0763636363636362</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1797,7 +1799,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
- finalize CAM - add classic drawing for TOP - recalculate VUVLO for new 1.2 schematics
</commit_message>
<xml_diff>
--- a/Preamp/Vuvlo_calc.xlsx
+++ b/Preamp/Vuvlo_calc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Vuvlo = Vbg * 1/(R1/R2)</t>
   </si>
@@ -30,12 +30,6 @@
     <t>Vbg = 1,21</t>
   </si>
   <si>
-    <t xml:space="preserve">Vuvlo3s = 9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vuvlo4s = 12  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Vuvlo5s = 15   </t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>MAX17562</t>
   </si>
   <si>
-    <t>4,7u</t>
-  </si>
-  <si>
     <t>35v</t>
   </si>
   <si>
@@ -118,6 +109,45 @@
   </si>
   <si>
     <t>2.4kOhm</t>
+  </si>
+  <si>
+    <t>OVLO</t>
+  </si>
+  <si>
+    <t>20u</t>
+  </si>
+  <si>
+    <t>100n</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vovlo = 24   </t>
+  </si>
+  <si>
+    <t>Target stop V</t>
+  </si>
+  <si>
+    <t>Stop V</t>
+  </si>
+  <si>
+    <t>4.2A (max)</t>
+  </si>
+  <si>
+    <t>3.6kOhm</t>
+  </si>
+  <si>
+    <t>3.3A</t>
+  </si>
+  <si>
+    <t>3.3kOhm</t>
+  </si>
+  <si>
+    <t>4.7kOhm</t>
+  </si>
+  <si>
+    <t>2.3A</t>
   </si>
 </sst>
 </file>
@@ -1612,10 +1642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1623,201 +1653,201 @@
     <col min="5" max="5" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3">
+        <v>24</v>
+      </c>
+      <c r="M3" s="1">
+        <f>$B$6*(1 + $B$5/L3)</f>
+        <v>21.2</v>
+      </c>
+      <c r="N3" s="1">
+        <v>20</v>
+      </c>
+      <c r="O3" s="1">
+        <f>$B$6*(1 + $B$5/N3)</f>
+        <v>25.2</v>
+      </c>
+      <c r="R3" t="e">
+        <f>N3/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
       <c r="B5">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>1.2</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D10" s="1">
-        <f>$B$5*$B$6/C10</f>
-        <v>52</v>
+        <f>$B$6*(1 + $B$5/C10)</f>
+        <v>33.200000000000003</v>
       </c>
       <c r="E10">
-        <f>D10/B12</f>
-        <v>10.4</v>
-      </c>
-      <c r="F10">
-        <v>53</v>
-      </c>
-      <c r="G10" s="1">
-        <f>$B$6*(1 + $B$5/F10)</f>
-        <v>10.030188679245283</v>
-      </c>
-      <c r="H10">
-        <f>G10/B10</f>
-        <v>3.3433962264150945</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>12</v>
-      </c>
-      <c r="D11" s="1">
-        <f t="shared" ref="D11:D12" si="0">$B$5*$B$6/C11</f>
+        <v>33</v>
+      </c>
+      <c r="F10" s="1">
+        <f>$B$6*(1 + $B$5/E10)</f>
+        <v>15.745454545454544</v>
+      </c>
+      <c r="G10">
+        <f>F10/B10</f>
+        <v>3.1490909090909089</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="D11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
         <v>39</v>
       </c>
-      <c r="E11">
-        <f>D11/B11</f>
-        <v>9.75</v>
-      </c>
-      <c r="F11">
-        <v>43</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" ref="G11:G12" si="1">$B$6*(1 + $B$5/F11)</f>
-        <v>12.083720930232557</v>
-      </c>
-      <c r="H11">
-        <f>G11/B11</f>
-        <v>3.0209302325581393</v>
-      </c>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>15</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>31.2</v>
-      </c>
-      <c r="E12">
-        <f>D12/B10</f>
-        <v>10.4</v>
-      </c>
-      <c r="F12">
-        <v>33</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" si="1"/>
-        <v>15.381818181818181</v>
-      </c>
-      <c r="H12">
-        <f>G12/B12</f>
-        <v>3.0763636363636362</v>
-      </c>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>33</v>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1839,17 +1869,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -1857,7 +1887,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <f>B3/(B6-1)</f>
@@ -1866,7 +1896,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>9.33</v>
@@ -1874,24 +1904,24 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>